<commit_message>
Added Form Link to Messenger Bot
</commit_message>
<xml_diff>
--- a/src/data/shop_list.xlsx
+++ b/src/data/shop_list.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeljose/Desktop/Coding Projects/javascript/goldieBot/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{745344B6-F744-0A4F-9B11-29C5BA37E64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14003C-0020-8246-AE9A-8CE9D125FBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CEA05502-54F0-624B-A8D6-28000A8B1EA3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{CEA05502-54F0-624B-A8D6-28000A8B1EA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Index</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Juice Box (Orange)</t>
   </si>
   <si>
-    <t>Juice Box (Tropical)</t>
-  </si>
-  <si>
     <t>Redbull</t>
   </si>
   <si>
-    <t>Oat Milk</t>
-  </si>
-  <si>
     <t>Coke (No Sugar) (Cold)</t>
   </si>
   <si>
@@ -112,30 +106,15 @@
     <t>Fanta</t>
   </si>
   <si>
-    <t>Kirk's Creaming Soda</t>
-  </si>
-  <si>
-    <t>Kirk's Creaming Soda (Cold)</t>
-  </si>
-  <si>
     <t>Redbull (Cold)</t>
   </si>
   <si>
     <t>Zooper Dooper</t>
   </si>
   <si>
-    <t>Rainbow Paddle Pops</t>
-  </si>
-  <si>
-    <t>Connoisseur (Cookies n' Cream)</t>
-  </si>
-  <si>
     <t>Connoisseur Mini (Cookies n' Cream)</t>
   </si>
   <si>
-    <t>Magnum Ice Cream</t>
-  </si>
-  <si>
     <t>Chupa Chups Bites</t>
   </si>
   <si>
@@ -172,9 +151,6 @@
     <t>Pringles (Sour Cream &amp; Onion)</t>
   </si>
   <si>
-    <t>Honey Soy Chips (Medium)</t>
-  </si>
-  <si>
     <t>Oreo Mini's</t>
   </si>
   <si>
@@ -251,6 +227,45 @@
   </si>
   <si>
     <t>Toilet Paper (Roll)</t>
+  </si>
+  <si>
+    <t>Connoisseur (Vanilla)</t>
+  </si>
+  <si>
+    <t>Connoisseur (Fudge)</t>
+  </si>
+  <si>
+    <t>Golden Gaytime</t>
+  </si>
+  <si>
+    <t>Milk (Skim)</t>
+  </si>
+  <si>
+    <t>Crunchie</t>
+  </si>
+  <si>
+    <t>Mars Pods</t>
+  </si>
+  <si>
+    <t>Red Rock Deli (Medium)</t>
+  </si>
+  <si>
+    <t>Red Rock Deli (Large)</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Yopro (Blueberry)</t>
+  </si>
+  <si>
+    <t>Yopro (Strawberry)</t>
+  </si>
+  <si>
+    <t>Reese's Bag</t>
+  </si>
+  <si>
+    <t>Caramel Crowns</t>
   </si>
 </sst>
 </file>
@@ -669,15 +684,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA681A1-A604-C846-BECC-CB18497791E7}">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
@@ -708,7 +723,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <f t="shared" ref="A3:A66" si="0">ROW(A2)</f>
+        <f t="shared" ref="A3:A71" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -748,22 +763,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C6" s="6">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A6)</f>
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -772,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6">
         <v>0.5</v>
@@ -784,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6">
         <v>0.5</v>
@@ -792,14 +807,14 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A9)</f>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -808,10 +823,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6">
         <v>1.5</v>
@@ -832,7 +847,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6">
         <v>1.5</v>
@@ -844,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6">
         <v>1.5</v>
@@ -856,7 +871,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6">
         <v>1.5</v>
@@ -868,7 +883,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6">
         <v>1.5</v>
@@ -880,7 +895,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6">
         <v>1.5</v>
@@ -892,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6">
         <v>1.5</v>
@@ -904,7 +919,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="6">
         <v>1.5</v>
@@ -916,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="6">
         <v>1.5</v>
@@ -928,7 +943,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="6">
         <v>1.5</v>
@@ -940,7 +955,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="7">
         <v>1.5</v>
@@ -948,11 +963,11 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A23:A28" si="1">ROW(A22)</f>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="7">
         <v>1.5</v>
@@ -960,62 +975,62 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1.5</v>
+        <v>24</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="7">
-        <v>1.5</v>
+      <c r="C25" s="6">
+        <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C26" s="6">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C27" s="6">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C28" s="6">
-        <v>0.6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1024,10 +1039,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" s="6">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1036,10 +1051,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="6">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1048,10 +1063,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C31" s="6">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1060,79 +1075,79 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="6">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A33:A41" si="2">ROW(A32)</f>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C33" s="6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C34" s="6">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C35" s="6">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C36" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C37" s="6">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C38" s="6">
         <v>2.5</v>
@@ -1140,35 +1155,35 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C39" s="6">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C40" s="6">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C41" s="6">
         <v>3</v>
@@ -1180,19 +1195,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C42" s="6">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
-        <f>ROW(A42)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C43" s="6">
         <v>1.5</v>
@@ -1204,46 +1219,46 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C44" s="6">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A44)</f>
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C45" s="6">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A45)</f>
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C46" s="6">
-        <v>0.4</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A46)</f>
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C47" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1252,10 +1267,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C48" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1264,10 +1279,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C49" s="6">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,10 +1291,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C50" s="6">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1288,10 +1303,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C51" s="6">
-        <v>1.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1300,10 +1315,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C52" s="6">
-        <v>2</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1312,10 +1327,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C53" s="6">
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1324,10 +1339,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C54" s="6">
-        <v>0.6</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,22 +1351,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C55" s="6">
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
-        <f t="shared" si="0"/>
+        <f>ROW(A55)</f>
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C56" s="6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1360,10 +1375,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C57" s="6">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,10 +1387,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C58" s="6">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1384,10 +1399,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C59" s="6">
-        <v>1.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1396,10 +1411,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C60" s="6">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,34 +1423,34 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C61" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <f>ROW(A60)</f>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C62" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
-        <f t="shared" si="0"/>
-        <v>62</v>
+        <f>ROW(A60)</f>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C63" s="6">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1444,10 +1459,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C64" s="6">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1456,10 +1471,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C65" s="6">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,57 +1483,117 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C66" s="6">
-        <v>2.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
-        <f t="shared" ref="A67:A70" si="1">ROW(A66)</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C67" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C68" s="6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C69" s="6">
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <f t="shared" ref="A72:A75" si="3">ROW(A71)</f>
         <v>71</v>
       </c>
-      <c r="C70" s="6">
+      <c r="B72" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" s="6">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>